<commit_message>
Small performance optimization, bugfix, usage update and result update
</commit_message>
<xml_diff>
--- a/exp_data.xlsx
+++ b/exp_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/albertan/Documents/CS561/561-final-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9EAF89C-BE41-894D-8C8F-7AA6233EAFA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95270636-8F22-AC4C-BF29-CE63B2A27A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="19740" windowHeight="17360" xr2:uid="{998DBC60-43D9-6541-9B99-4C5C65020B43}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22380" windowHeight="26400" xr2:uid="{998DBC60-43D9-6541-9B99-4C5C65020B43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -262,32 +262,26 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$16:$B$23</c:f>
+              <c:f>Sheet1!$B$18:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>300</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>700</c:v>
-                </c:pt>
-                <c:pt idx="7">
                   <c:v>1000</c:v>
                 </c:pt>
               </c:numCache>
@@ -295,33 +289,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$16:$D$23</c:f>
+              <c:f>Sheet1!$D$18:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>25430</c:v>
+                  <c:v>7402</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25330</c:v>
+                  <c:v>7338</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23644</c:v>
+                  <c:v>6366</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23621</c:v>
+                  <c:v>6318</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21673</c:v>
+                  <c:v>6604</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22965</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>23779</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>25446</c:v>
+                  <c:v>6717</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -791,6 +779,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Leveling</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -805,10 +796,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$8</c:f>
+              <c:f>Sheet1!$A$3:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -816,43 +807,37 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>100</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>300</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$8</c:f>
+              <c:f>Sheet1!$D$3:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>24284</c:v>
+                  <c:v>8230</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21187</c:v>
+                  <c:v>7080</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20523</c:v>
+                  <c:v>6574</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21220</c:v>
+                  <c:v>6728</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21612</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>27791</c:v>
+                  <c:v>7006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -861,6 +846,79 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-1398-0843-8DAD-66EABC7B84FE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Tiering</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$3:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>11888</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10893</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12551</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12595</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16928</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F213-C749-8683-54A801506C7F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1149,6 +1207,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1228,7 +1317,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-CN" sz="1800"/>
-              <a:t>Reading</a:t>
+              <a:t>Reading-predominant</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="zh-CN" altLang="en-US" sz="1800"/>
@@ -1236,7 +1325,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-CN" sz="1800"/>
-              <a:t>Priority</a:t>
+              <a:t>Operations</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="1800"/>
           </a:p>
@@ -1589,15 +1678,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-CN" sz="1800"/>
-              <a:t>Writing</a:t>
+              <a:t>Writing-predominant</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="zh-CN" altLang="en-US" sz="1800"/>
+              <a:rPr lang="zh-CN" altLang="en-US" sz="1800" baseline="0"/>
               <a:t> </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN" sz="1800"/>
-              <a:t>Priority</a:t>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1800" baseline="0"/>
+              <a:t>Operations</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="1800"/>
           </a:p>
@@ -1721,6 +1810,1022 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2019910063"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2019910063"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" sz="1400"/>
+                  <a:t>Time/ms</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2020207823"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="2400"/>
+              <a:t>BF</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US" sz="2400" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="2400" baseline="0"/>
+              <a:t>Affects</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US" sz="2400" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="2400" baseline="0"/>
+              <a:t>on</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US" sz="2400" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="2400" baseline="0"/>
+              <a:t>Database</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US" sz="2400" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="2400" baseline="0"/>
+              <a:t>Performance</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="2400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>bitsPerElement = 64</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$19:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$19:$D$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>7338</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6366</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6318</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6604</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6717</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9642-6344-93F7-E57DF2882D12}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>bitsPerElement = 8</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$19:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$19:$E$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>7648</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6488</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6529</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6764</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6988</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-9642-6344-93F7-E57DF2882D12}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="764904671"/>
+        <c:axId val="764980591"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="764904671"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" sz="1800"/>
+                  <a:t>First</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="zh-CN" altLang="en-US" sz="1800"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" sz="1800"/>
+                  <a:t>Level</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="zh-CN" altLang="en-US" sz="1800"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" sz="1800"/>
+                  <a:t>Threshold</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1800"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="764980591"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="764980591"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" sz="1800"/>
+                  <a:t>Time/ms</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1800"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="764904671"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1800"/>
+              <a:t>Key</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US" sz="1800"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1800"/>
+              <a:t>Distribution</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1800"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$36:$A$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$36:$B$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2045</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7402</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20413</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A7EA-A74A-B05C-0AAC327B967D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="2020207823"/>
+        <c:axId val="2019910063"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2020207823"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" sz="1800"/>
+                  <a:t>Max</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="zh-CN" altLang="en-US" sz="1800"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" sz="1800"/>
+                  <a:t>Key</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1800"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2089,6 +3194,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -3625,6 +4810,1025 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4133,14 +6337,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4167,16 +6371,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4206,15 +6410,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4242,15 +6446,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4272,6 +6476,80 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2FD8DC4-D90B-AF46-A065-7F3680D4A84A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF72D15B-DF5E-8147-B01D-44CEB6B242E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4577,15 +6855,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F58305B-6E20-5047-80F0-5E7326230F12}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="M97" sqref="M97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -4596,7 +6874,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4610,203 +6888,194 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>5</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="D3">
-        <v>24284</v>
+        <v>8230</v>
+      </c>
+      <c r="E3">
+        <v>11888</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>10</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="D4">
-        <v>21187</v>
+        <v>7080</v>
+      </c>
+      <c r="E4">
+        <v>10893</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>25</v>
+      </c>
+      <c r="C5">
+        <v>25</v>
+      </c>
+      <c r="D5">
+        <v>6574</v>
+      </c>
+      <c r="E5">
+        <v>12551</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>50</v>
       </c>
-      <c r="B5">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>20523</v>
+      <c r="B6">
+        <v>25</v>
+      </c>
+      <c r="C6">
+        <v>25</v>
+      </c>
+      <c r="D6">
+        <v>6728</v>
+      </c>
+      <c r="E6">
+        <v>12595</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>100</v>
-      </c>
-      <c r="B6">
-        <v>10</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>21220</v>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>75</v>
+      </c>
+      <c r="B7">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <v>25</v>
+      </c>
+      <c r="D7">
+        <v>7006</v>
+      </c>
+      <c r="E7">
+        <v>16928</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>150</v>
-      </c>
-      <c r="B7">
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7">
-        <v>21612</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>300</v>
-      </c>
-      <c r="B8">
-        <v>10</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8">
-        <v>27791</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>5</v>
-      </c>
-      <c r="B16">
-        <v>5</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-      <c r="D16">
-        <v>25430</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>5</v>
-      </c>
-      <c r="B17">
-        <v>10</v>
-      </c>
-      <c r="C17">
-        <v>3</v>
-      </c>
-      <c r="D17">
-        <v>25330</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B18">
         <v>50</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="D18">
-        <v>23644</v>
+        <v>7402</v>
+      </c>
+      <c r="E18">
+        <v>8604</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B19">
         <v>100</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="D19">
-        <v>23621</v>
+        <v>7338</v>
+      </c>
+      <c r="E19">
+        <v>7648</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B20">
         <v>300</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="D20">
-        <v>21673</v>
+        <v>6366</v>
+      </c>
+      <c r="E20">
+        <v>6488</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B21">
         <v>500</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="D21">
-        <v>22965</v>
+        <v>6318</v>
+      </c>
+      <c r="E21">
+        <v>6529</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B22">
         <v>700</v>
       </c>
       <c r="C22">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="D22">
-        <v>23779</v>
+        <v>6604</v>
+      </c>
+      <c r="E22">
+        <v>6764</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B23">
         <v>1000</v>
       </c>
       <c r="C23">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="D23">
-        <v>25446</v>
+        <v>6717</v>
+      </c>
+      <c r="E23">
+        <v>6988</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>8</v>
       </c>
@@ -4814,7 +7083,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -4825,7 +7094,7 @@
         <v>100.9</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -4834,6 +7103,30 @@
       </c>
       <c r="C29">
         <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>200</v>
+      </c>
+      <c r="B36">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>2000</v>
+      </c>
+      <c r="B37">
+        <v>7402</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>10000</v>
+      </c>
+      <c r="B38">
+        <v>20413</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add comment, report, slides, and update data results
</commit_message>
<xml_diff>
--- a/exp_data.xlsx
+++ b/exp_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/albertan/Documents/CS561/561-final-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95270636-8F22-AC4C-BF29-CE63B2A27A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410415FA-82D4-0043-BD87-AC6DE3838FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="22380" windowHeight="26400" xr2:uid="{998DBC60-43D9-6541-9B99-4C5C65020B43}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21480" windowHeight="26400" xr2:uid="{998DBC60-43D9-6541-9B99-4C5C65020B43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -294,22 +294,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>7402</c:v>
+                  <c:v>8702</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7338</c:v>
+                  <c:v>9024</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6366</c:v>
+                  <c:v>7336</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6318</c:v>
+                  <c:v>7417</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6604</c:v>
+                  <c:v>7674</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6717</c:v>
+                  <c:v>7930</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1401,10 +1401,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>17524</c:v>
+                  <c:v>4538</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26206</c:v>
+                  <c:v>7556</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1737,10 +1737,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>100.9</c:v>
+                  <c:v>1619</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>66</c:v>
+                  <c:v>308.6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1776,10 +1776,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>100.9</c:v>
+                  <c:v>1619</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>66</c:v>
+                  <c:v>308.60000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2175,19 +2175,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>7338</c:v>
+                  <c:v>9024</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6366</c:v>
+                  <c:v>7336</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6318</c:v>
+                  <c:v>7417</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6604</c:v>
+                  <c:v>7674</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6717</c:v>
+                  <c:v>7930</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2248,19 +2248,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>7648</c:v>
+                  <c:v>9000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6488</c:v>
+                  <c:v>7321</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6529</c:v>
+                  <c:v>7333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6764</c:v>
+                  <c:v>7498</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6988</c:v>
+                  <c:v>7849</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6857,8 +6857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F58305B-6E20-5047-80F0-5E7326230F12}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="M97" sqref="M97"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6973,6 +6973,14 @@
         <v>16928</v>
       </c>
     </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>10</v>
+      </c>
+    </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>50</v>
@@ -6984,10 +6992,10 @@
         <v>25</v>
       </c>
       <c r="D18">
-        <v>7402</v>
+        <v>8702</v>
       </c>
       <c r="E18">
-        <v>8604</v>
+        <v>8658</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -7001,10 +7009,10 @@
         <v>25</v>
       </c>
       <c r="D19">
-        <v>7338</v>
+        <v>9024</v>
       </c>
       <c r="E19">
-        <v>7648</v>
+        <v>9000</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -7018,10 +7026,10 @@
         <v>25</v>
       </c>
       <c r="D20">
-        <v>6366</v>
+        <v>7336</v>
       </c>
       <c r="E20">
-        <v>6488</v>
+        <v>7321</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -7035,10 +7043,10 @@
         <v>25</v>
       </c>
       <c r="D21">
-        <v>6318</v>
+        <v>7417</v>
       </c>
       <c r="E21">
-        <v>6529</v>
+        <v>7333</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -7052,10 +7060,10 @@
         <v>25</v>
       </c>
       <c r="D22">
-        <v>6604</v>
+        <v>7674</v>
       </c>
       <c r="E22">
-        <v>6764</v>
+        <v>7498</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -7069,10 +7077,10 @@
         <v>25</v>
       </c>
       <c r="D23">
-        <v>6717</v>
+        <v>7930</v>
       </c>
       <c r="E23">
-        <v>6988</v>
+        <v>7849</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -7088,10 +7096,10 @@
         <v>4</v>
       </c>
       <c r="B28">
-        <v>17524</v>
+        <v>4538</v>
       </c>
       <c r="C28">
-        <v>100.9</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -7099,10 +7107,10 @@
         <v>5</v>
       </c>
       <c r="B29">
-        <v>26206</v>
+        <v>7556</v>
       </c>
       <c r="C29">
-        <v>66</v>
+        <v>308.60000000000002</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>